<commit_message>
Slight update to species thresholds
</commit_message>
<xml_diff>
--- a/manuscript_code/Data/SpeciesThresholds.xlsx
+++ b/manuscript_code/Data/SpeciesThresholds.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://doimspp-my.sharepoint.com/personal/cpien_usbr_gov/Documents/Work/WaterTemp/TempSynthesis/SpeciesTables/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://doimspp-my.sharepoint.com/personal/cpien_usbr_gov/Documents/Work/WaterTemp/TempSynthesis/manuscript_code/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="99" documentId="8_{2681606B-0122-416A-9508-511D19A4BC48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3A8CA11B-59A3-4912-9542-880E91A3BC55}"/>
+  <xr:revisionPtr revIDLastSave="100" documentId="8_{2681606B-0122-416A-9508-511D19A4BC48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9F248B82-60B0-47F5-8258-6614D57708CB}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F95700F2-2543-4D53-85A7-DBBD5FF11025}"/>
   </bookViews>
@@ -320,9 +320,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -360,7 +360,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -466,7 +466,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -608,7 +608,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -620,7 +620,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D53" sqref="D53"/>
+      <selection pane="bottomLeft" activeCell="H47" sqref="H47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1923,7 +1923,7 @@
         <v>30</v>
       </c>
       <c r="F50" s="6">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="G50" s="6">
         <v>30</v>

</xml_diff>